<commit_message>
Consequently number the test case variables
The originally proposed numbering was not supported by PHP (variables
cannot start with a numeric value).

(cherry picked from commit 3da40a0)
</commit_message>
<xml_diff>
--- a/docs/testmatrix-stepup-gateway-loa.xlsx
+++ b/docs/testmatrix-stepup-gateway-loa.xlsx
@@ -31,8 +31,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1a. No sp-institution specific configuration provided (i.e. </t>
+      <t xml:space="preserve">a1. No sp-institution specific configuration provided (i.e. </t>
     </r>
     <r>
       <rPr>
@@ -40,6 +41,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">__default__</t>
     </r>
@@ -49,6 +51,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> = LoA 1)</t>
     </r>
@@ -60,8 +63,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1b. An sp-institution specific configuration is provided for institution </t>
+      <t xml:space="preserve">a2. An sp-institution specific configuration is provided for institution </t>
     </r>
     <r>
       <rPr>
@@ -69,6 +73,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;A&gt;</t>
     </r>
@@ -78,6 +83,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> with a LoA = 2</t>
     </r>
@@ -89,8 +95,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2a. The user has schacHomeOrganization attribute set to </t>
+      <t xml:space="preserve">a3. The user has schacHomeOrganization attribute set to </t>
     </r>
     <r>
       <rPr>
@@ -98,6 +105,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;A&gt;</t>
     </r>
@@ -109,8 +117,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2b. The user has schacHomeOrganization attribute set to </t>
+      <t xml:space="preserve">b1. The user has schacHomeOrganization attribute set to </t>
     </r>
     <r>
       <rPr>
@@ -118,6 +127,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;A&gt;</t>
     </r>
@@ -127,36 +137,37 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, but the case does not match</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">2c. The user has no schacHomeOrganization attribute set</t>
+    <t xml:space="preserve">b2. The user has no schacHomeOrganization attribute set</t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">2d. The user has a schacHomeOrganization attribute set that is different from the one used during registration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3a. The user has a vetted token (i.e. NameID exists in the second_factor table)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3b. The user does not not have a vetted token</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4a. SP does not request a LoA (i.e. no AuthContexClassRef in AuthnRequest)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4b. SP requests LoA = 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4c. SP requests LoA = 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4c. SP requests LoA = 3</t>
+    <t xml:space="preserve">b3. The user has a schacHomeOrganization attribute set that is different from the one used during registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c1. The user has a vetted token (i.e. NameID exists in the second_factor table)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c2. The user does not not have a vetted token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1. SP does not request a LoA (i.e. no AuthContexClassRef in AuthnRequest)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d2. SP requests LoA = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d3. SP requests LoA = 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d4. SP requests LoA = 3</t>
   </si>
   <si>
     <t xml:space="preserve">Resulting Required LoA</t>
@@ -193,6 +204,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -215,18 +227,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -234,24 +249,28 @@
       <color rgb="FF808080"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -259,6 +278,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -266,30 +286,35 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF808080"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -297,6 +322,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -304,6 +330,7 @@
       <color rgb="FF808080"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -574,7 +601,7 @@
   <dimension ref="A1:BM21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BK17" activeCellId="0" sqref="BK17"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>